<commit_message>
met de sieve methode
</commit_message>
<xml_diff>
--- a/efficiency.xlsx
+++ b/efficiency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\Qien\Eclipse Workspace\Primes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91878DC7-854B-46A8-8952-82E2562E3D4C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1335BE-68F7-44A7-BB73-F7B46552571D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{54A8314F-1F24-4809-946A-AF7827222D93}"/>
+    <workbookView xWindow="14040" yWindow="1644" windowWidth="17280" windowHeight="8964" xr2:uid="{54A8314F-1F24-4809-946A-AF7827222D93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>